<commit_message>
Nuevos cambios por filas y por columnas
</commit_message>
<xml_diff>
--- a/PRUEBA_ESPECIAL.xlsx
+++ b/PRUEBA_ESPECIAL.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve">Titulo11</t>
   </si>
   <si>
-    <t xml:space="preserve">Titulo12</t>
+    <t xml:space="preserve">Titulo12_grafico</t>
   </si>
   <si>
     <t xml:space="preserve">Titulo13</t>
@@ -188,7 +188,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
     <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-      <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">27</xdr:col>
+      <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">29</xdr:col>
       <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
       <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">34</xdr:row>
       <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
@@ -220,8 +220,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="S134:T184" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="S134:T184"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="T134:U184" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="T134:U184"/>
   <tableColumns count="2">
     <tableColumn id="1" name="speed"/>
     <tableColumn id="2" name="dist"/>
@@ -231,8 +231,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="AB2:AN13" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="AB2:AN13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="AD2:AP13" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="AD2:AP13"/>
   <tableColumns count="13">
     <tableColumn id="1" name="vars"/>
     <tableColumn id="2" name="n"/>
@@ -253,8 +253,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="AB19:AN29" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="AB19:AN29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="AD19:AP29" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="AD19:AP29"/>
   <tableColumns count="13">
     <tableColumn id="1" name="vars"/>
     <tableColumn id="2" name="n"/>
@@ -275,8 +275,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="AB60:AC110" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="AB60:AC110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="AD60:AE110" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="AD60:AE110"/>
   <tableColumns count="2">
     <tableColumn id="1" name="speed"/>
     <tableColumn id="2" name="dist"/>
@@ -341,8 +341,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="S2:V4" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="S2:V4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="T2:W4" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="T2:W4"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Estimate"/>
     <tableColumn id="2" name="Std. Error"/>
@@ -354,8 +354,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="S10:V16" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="S10:V16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="T10:W16" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="T10:W16"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Estimate"/>
     <tableColumn id="2" name="Std. Error"/>
@@ -367,8 +367,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="S22:T72" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="S22:T72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="T22:U72" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="T22:U72"/>
   <tableColumns count="2">
     <tableColumn id="1" name="speed"/>
     <tableColumn id="2" name="dist"/>
@@ -378,8 +378,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="S78:T128" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="S78:T128"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="T78:U128" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="T78:U128"/>
   <tableColumns count="2">
     <tableColumn id="1" name="speed"/>
     <tableColumn id="2" name="dist"/>
@@ -677,10 +677,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -724,55 +724,55 @@
       <c r="M2" t="s">
         <v>13</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>20</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>21</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>22</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>1</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>2</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
         <v>3</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>5</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AI2" t="s">
         <v>6</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AJ2" t="s">
         <v>7</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AK2" t="s">
         <v>8</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>9</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AM2" t="s">
         <v>10</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AN2" t="s">
         <v>11</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AO2" t="s">
         <v>12</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AP2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -816,55 +816,55 @@
       <c r="M3" t="n">
         <v>1.06542395937281</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>12.3033741559962</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>18.7178844287215</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>0.657305808402012</v>
       </c>
-      <c r="V3" t="n">
+      <c r="W3" t="n">
         <v>0.518124396898475</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AD3" t="n">
         <v>1</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AE3" t="n">
         <v>32</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AF3" t="n">
         <v>20.090625</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AG3" t="n">
         <v>6.0269480520891</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="AH3" t="n">
         <v>19.2</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="AI3" t="n">
         <v>19.6961538461538</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="AJ3" t="n">
         <v>5.41149</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="AK3" t="n">
         <v>10.4</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="AL3" t="n">
         <v>33.9</v>
       </c>
-      <c r="AK3" t="n">
+      <c r="AM3" t="n">
         <v>23.5</v>
       </c>
-      <c r="AL3" t="n">
+      <c r="AN3" t="n">
         <v>0.610655017573288</v>
       </c>
-      <c r="AM3" t="n">
+      <c r="AO3" t="n">
         <v>-0.372766029820891</v>
       </c>
-      <c r="AN3" t="n">
+      <c r="AP3" t="n">
         <v>1.06542395937281</v>
       </c>
     </row>
@@ -908,55 +908,55 @@
       <c r="M4" t="n">
         <v>0.315709326805937</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>0.655413017081793</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>1.4932599610728</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>0.438914210631434</v>
       </c>
-      <c r="V4" t="n">
+      <c r="W4" t="n">
         <v>0.665206434293021</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AD4" t="n">
         <v>2</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AE4" t="n">
         <v>32</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AF4" t="n">
         <v>6.1875</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AG4" t="n">
         <v>1.78592164694654</v>
       </c>
-      <c r="AF4" t="n">
+      <c r="AH4" t="n">
         <v>6</v>
       </c>
-      <c r="AG4" t="n">
+      <c r="AI4" t="n">
         <v>6.23076923076923</v>
       </c>
-      <c r="AH4" t="n">
+      <c r="AJ4" t="n">
         <v>2.9652</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>4</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>8</v>
       </c>
       <c r="AK4" t="n">
         <v>4</v>
       </c>
       <c r="AL4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN4" t="n">
         <v>-0.174611913930169</v>
       </c>
-      <c r="AM4" t="n">
+      <c r="AO4" t="n">
         <v>-1.76211977398177</v>
       </c>
-      <c r="AN4" t="n">
+      <c r="AP4" t="n">
         <v>0.315709326805937</v>
       </c>
     </row>
@@ -1000,43 +1000,43 @@
       <c r="M5" t="n">
         <v>21.9094727148934</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AD5" t="n">
         <v>3</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AE5" t="n">
         <v>32</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AF5" t="n">
         <v>230.721875</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AG5" t="n">
         <v>123.938693831382</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AH5" t="n">
         <v>196.3</v>
       </c>
-      <c r="AG5" t="n">
+      <c r="AI5" t="n">
         <v>222.523076923077</v>
       </c>
-      <c r="AH5" t="n">
+      <c r="AJ5" t="n">
         <v>140.47635</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AK5" t="n">
         <v>71.1</v>
       </c>
-      <c r="AJ5" t="n">
+      <c r="AL5" t="n">
         <v>472</v>
       </c>
-      <c r="AK5" t="n">
+      <c r="AM5" t="n">
         <v>400.9</v>
       </c>
-      <c r="AL5" t="n">
+      <c r="AN5" t="n">
         <v>0.381657034147599</v>
       </c>
-      <c r="AM5" t="n">
+      <c r="AO5" t="n">
         <v>-1.2072119466699</v>
       </c>
-      <c r="AN5" t="n">
+      <c r="AP5" t="n">
         <v>21.9094727148934</v>
       </c>
     </row>
@@ -1080,43 +1080,43 @@
       <c r="M6" t="n">
         <v>12.1203173116</v>
       </c>
-      <c r="AB6" t="n">
+      <c r="AD6" t="n">
         <v>4</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AE6" t="n">
         <v>32</v>
       </c>
-      <c r="AD6" t="n">
+      <c r="AF6" t="n">
         <v>146.6875</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="AG6" t="n">
         <v>68.5628684893206</v>
       </c>
-      <c r="AF6" t="n">
+      <c r="AH6" t="n">
         <v>123</v>
       </c>
-      <c r="AG6" t="n">
+      <c r="AI6" t="n">
         <v>141.192307692308</v>
       </c>
-      <c r="AH6" t="n">
+      <c r="AJ6" t="n">
         <v>77.0952</v>
       </c>
-      <c r="AI6" t="n">
+      <c r="AK6" t="n">
         <v>52</v>
       </c>
-      <c r="AJ6" t="n">
+      <c r="AL6" t="n">
         <v>335</v>
       </c>
-      <c r="AK6" t="n">
+      <c r="AM6" t="n">
         <v>283</v>
       </c>
-      <c r="AL6" t="n">
+      <c r="AN6" t="n">
         <v>0.726023656361273</v>
       </c>
-      <c r="AM6" t="n">
+      <c r="AO6" t="n">
         <v>-0.135551121097421</v>
       </c>
-      <c r="AN6" t="n">
+      <c r="AP6" t="n">
         <v>12.1203173116</v>
       </c>
     </row>
@@ -1160,43 +1160,43 @@
       <c r="M7" t="n">
         <v>0.0945187400080091</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AD7" t="n">
         <v>5</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AE7" t="n">
         <v>32</v>
       </c>
-      <c r="AD7" t="n">
+      <c r="AF7" t="n">
         <v>3.5965625</v>
       </c>
-      <c r="AE7" t="n">
+      <c r="AG7" t="n">
         <v>0.534678736070971</v>
       </c>
-      <c r="AF7" t="n">
+      <c r="AH7" t="n">
         <v>3.695</v>
       </c>
-      <c r="AG7" t="n">
+      <c r="AI7" t="n">
         <v>3.57923076923077</v>
       </c>
-      <c r="AH7" t="n">
+      <c r="AJ7" t="n">
         <v>0.704235</v>
       </c>
-      <c r="AI7" t="n">
+      <c r="AK7" t="n">
         <v>2.76</v>
       </c>
-      <c r="AJ7" t="n">
+      <c r="AL7" t="n">
         <v>4.93</v>
       </c>
-      <c r="AK7" t="n">
+      <c r="AM7" t="n">
         <v>2.17</v>
       </c>
-      <c r="AL7" t="n">
+      <c r="AN7" t="n">
         <v>0.265903904603492</v>
       </c>
-      <c r="AM7" t="n">
+      <c r="AO7" t="n">
         <v>-0.714700615734489</v>
       </c>
-      <c r="AN7" t="n">
+      <c r="AP7" t="n">
         <v>0.0945187400080091</v>
       </c>
     </row>
@@ -1240,43 +1240,43 @@
       <c r="M8" t="n">
         <v>0.172968473260116</v>
       </c>
-      <c r="AB8" t="n">
+      <c r="AD8" t="n">
         <v>6</v>
       </c>
-      <c r="AC8" t="n">
+      <c r="AE8" t="n">
         <v>32</v>
       </c>
-      <c r="AD8" t="n">
+      <c r="AF8" t="n">
         <v>3.21725</v>
       </c>
-      <c r="AE8" t="n">
+      <c r="AG8" t="n">
         <v>0.978457442989697</v>
       </c>
-      <c r="AF8" t="n">
+      <c r="AH8" t="n">
         <v>3.325</v>
       </c>
-      <c r="AG8" t="n">
+      <c r="AI8" t="n">
         <v>3.15269230769231</v>
       </c>
-      <c r="AH8" t="n">
+      <c r="AJ8" t="n">
         <v>0.7672455</v>
       </c>
-      <c r="AI8" t="n">
+      <c r="AK8" t="n">
         <v>1.513</v>
       </c>
-      <c r="AJ8" t="n">
+      <c r="AL8" t="n">
         <v>5.424</v>
       </c>
-      <c r="AK8" t="n">
+      <c r="AM8" t="n">
         <v>3.911</v>
       </c>
-      <c r="AL8" t="n">
+      <c r="AN8" t="n">
         <v>0.423146464177225</v>
       </c>
-      <c r="AM8" t="n">
+      <c r="AO8" t="n">
         <v>-0.0227107528393127</v>
       </c>
-      <c r="AN8" t="n">
+      <c r="AP8" t="n">
         <v>0.172968473260116</v>
       </c>
     </row>
@@ -1320,46 +1320,46 @@
       <c r="M9" t="n">
         <v>0.315889919959878</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" t="n">
+      <c r="AD9" t="n">
         <v>7</v>
       </c>
-      <c r="AC9" t="n">
+      <c r="AE9" t="n">
         <v>32</v>
       </c>
-      <c r="AD9" t="n">
+      <c r="AF9" t="n">
         <v>17.84875</v>
       </c>
-      <c r="AE9" t="n">
+      <c r="AG9" t="n">
         <v>1.78694323609684</v>
       </c>
-      <c r="AF9" t="n">
+      <c r="AH9" t="n">
         <v>17.71</v>
       </c>
-      <c r="AG9" t="n">
+      <c r="AI9" t="n">
         <v>17.8276923076923</v>
       </c>
-      <c r="AH9" t="n">
+      <c r="AJ9" t="n">
         <v>1.415883</v>
       </c>
-      <c r="AI9" t="n">
+      <c r="AK9" t="n">
         <v>14.5</v>
       </c>
-      <c r="AJ9" t="n">
+      <c r="AL9" t="n">
         <v>22.9</v>
       </c>
-      <c r="AK9" t="n">
+      <c r="AM9" t="n">
         <v>8.4</v>
       </c>
-      <c r="AL9" t="n">
+      <c r="AN9" t="n">
         <v>0.369045278509436</v>
       </c>
-      <c r="AM9" t="n">
+      <c r="AO9" t="n">
         <v>0.335114219571393</v>
       </c>
-      <c r="AN9" t="n">
+      <c r="AP9" t="n">
         <v>0.315889919959878</v>
       </c>
     </row>
@@ -1403,55 +1403,55 @@
       <c r="M10" t="n">
         <v>0.0890983056209046</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>20</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>21</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>22</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>23</v>
       </c>
-      <c r="AB10" t="n">
+      <c r="AD10" t="n">
         <v>8</v>
       </c>
-      <c r="AC10" t="n">
+      <c r="AE10" t="n">
         <v>32</v>
       </c>
-      <c r="AD10" t="n">
+      <c r="AF10" t="n">
         <v>0.4375</v>
       </c>
-      <c r="AE10" t="n">
+      <c r="AG10" t="n">
         <v>0.504016128774185</v>
-      </c>
-      <c r="AF10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG10" t="n">
-        <v>0.423076923076923</v>
       </c>
       <c r="AH10" t="n">
         <v>0</v>
       </c>
       <c r="AI10" t="n">
+        <v>0.423076923076923</v>
+      </c>
+      <c r="AJ10" t="n">
         <v>0</v>
       </c>
-      <c r="AJ10" t="n">
+      <c r="AK10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL10" t="n">
         <v>1</v>
       </c>
-      <c r="AK10" t="n">
+      <c r="AM10" t="n">
         <v>1</v>
       </c>
-      <c r="AL10" t="n">
+      <c r="AN10" t="n">
         <v>0.240257688369044</v>
       </c>
-      <c r="AM10" t="n">
+      <c r="AO10" t="n">
         <v>-2.00193762400794</v>
       </c>
-      <c r="AN10" t="n">
+      <c r="AP10" t="n">
         <v>0.0890983056209046</v>
       </c>
     </row>
@@ -1495,55 +1495,55 @@
       <c r="M11" t="n">
         <v>0.0882099653319905</v>
       </c>
-      <c r="S11" t="n">
+      <c r="T11" t="n">
         <v>2.17126629215507</v>
       </c>
-      <c r="T11" t="n">
+      <c r="U11" t="n">
         <v>0.27979415471378</v>
       </c>
-      <c r="U11" t="n">
+      <c r="V11" t="n">
         <v>7.76022749430276</v>
       </c>
-      <c r="V11" t="n">
+      <c r="W11" t="n">
         <v>0.00000000000142950220581308</v>
       </c>
-      <c r="AB11" t="n">
+      <c r="AD11" t="n">
         <v>9</v>
       </c>
-      <c r="AC11" t="n">
+      <c r="AE11" t="n">
         <v>32</v>
       </c>
-      <c r="AD11" t="n">
+      <c r="AF11" t="n">
         <v>0.40625</v>
       </c>
-      <c r="AE11" t="n">
+      <c r="AG11" t="n">
         <v>0.498990917235846</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG11" t="n">
-        <v>0.384615384615385</v>
       </c>
       <c r="AH11" t="n">
         <v>0</v>
       </c>
       <c r="AI11" t="n">
+        <v>0.384615384615385</v>
+      </c>
+      <c r="AJ11" t="n">
         <v>0</v>
       </c>
-      <c r="AJ11" t="n">
+      <c r="AK11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL11" t="n">
         <v>1</v>
       </c>
-      <c r="AK11" t="n">
+      <c r="AM11" t="n">
         <v>1</v>
       </c>
-      <c r="AL11" t="n">
+      <c r="AN11" t="n">
         <v>0.364015894329692</v>
       </c>
-      <c r="AM11" t="n">
+      <c r="AO11" t="n">
         <v>-1.92474142839069</v>
       </c>
-      <c r="AN11" t="n">
+      <c r="AP11" t="n">
         <v>0.0882099653319905</v>
       </c>
     </row>
@@ -1587,55 +1587,55 @@
       <c r="M12" t="n">
         <v>0.130426564432547</v>
       </c>
-      <c r="S12" t="n">
+      <c r="T12" t="n">
         <v>0.495888938388551</v>
       </c>
-      <c r="T12" t="n">
+      <c r="U12" t="n">
         <v>0.0860699223088161</v>
       </c>
-      <c r="U12" t="n">
+      <c r="V12" t="n">
         <v>5.76146608578683</v>
       </c>
-      <c r="V12" t="n">
+      <c r="W12" t="n">
         <v>0.0000000486751586760195</v>
       </c>
-      <c r="AB12" t="n">
+      <c r="AD12" t="n">
         <v>10</v>
       </c>
-      <c r="AC12" t="n">
+      <c r="AE12" t="n">
         <v>32</v>
       </c>
-      <c r="AD12" t="n">
+      <c r="AF12" t="n">
         <v>3.6875</v>
       </c>
-      <c r="AE12" t="n">
+      <c r="AG12" t="n">
         <v>0.737804065256947</v>
       </c>
-      <c r="AF12" t="n">
+      <c r="AH12" t="n">
         <v>4</v>
       </c>
-      <c r="AG12" t="n">
+      <c r="AI12" t="n">
         <v>3.61538461538462</v>
       </c>
-      <c r="AH12" t="n">
+      <c r="AJ12" t="n">
         <v>1.4826</v>
       </c>
-      <c r="AI12" t="n">
+      <c r="AK12" t="n">
         <v>3</v>
       </c>
-      <c r="AJ12" t="n">
+      <c r="AL12" t="n">
         <v>5</v>
       </c>
-      <c r="AK12" t="n">
+      <c r="AM12" t="n">
         <v>2</v>
       </c>
-      <c r="AL12" t="n">
+      <c r="AN12" t="n">
         <v>0.52885446231085</v>
       </c>
-      <c r="AM12" t="n">
+      <c r="AO12" t="n">
         <v>-1.06975067515432</v>
       </c>
-      <c r="AN12" t="n">
+      <c r="AP12" t="n">
         <v>0.130426564432547</v>
       </c>
     </row>
@@ -1679,97 +1679,97 @@
       <c r="M13" t="n">
         <v>0.285529714288961</v>
       </c>
-      <c r="S13" t="n">
+      <c r="T13" t="n">
         <v>0.829243912234806</v>
       </c>
-      <c r="T13" t="n">
+      <c r="U13" t="n">
         <v>0.0685276454152499</v>
       </c>
-      <c r="U13" t="n">
+      <c r="V13" t="n">
         <v>12.100866843008</v>
       </c>
-      <c r="V13" t="n">
+      <c r="W13" t="n">
         <v>0.0000000000000000000000107359248017686</v>
       </c>
-      <c r="AB13" t="n">
+      <c r="AD13" t="n">
         <v>11</v>
       </c>
-      <c r="AC13" t="n">
+      <c r="AE13" t="n">
         <v>32</v>
       </c>
-      <c r="AD13" t="n">
+      <c r="AF13" t="n">
         <v>2.8125</v>
       </c>
-      <c r="AE13" t="n">
+      <c r="AG13" t="n">
         <v>1.61519997763185</v>
       </c>
-      <c r="AF13" t="n">
+      <c r="AH13" t="n">
         <v>2</v>
       </c>
-      <c r="AG13" t="n">
+      <c r="AI13" t="n">
         <v>2.65384615384615</v>
       </c>
-      <c r="AH13" t="n">
+      <c r="AJ13" t="n">
         <v>1.4826</v>
       </c>
-      <c r="AI13" t="n">
+      <c r="AK13" t="n">
         <v>1</v>
       </c>
-      <c r="AJ13" t="n">
+      <c r="AL13" t="n">
         <v>8</v>
       </c>
-      <c r="AK13" t="n">
+      <c r="AM13" t="n">
         <v>7</v>
       </c>
-      <c r="AL13" t="n">
+      <c r="AN13" t="n">
         <v>1.05087376449851</v>
       </c>
-      <c r="AM13" t="n">
+      <c r="AO13" t="n">
         <v>1.25704307347743</v>
       </c>
-      <c r="AN13" t="n">
+      <c r="AP13" t="n">
         <v>0.285529714288961</v>
       </c>
     </row>
     <row r="14">
-      <c r="S14" t="n">
+      <c r="T14" t="n">
         <v>-0.315155173326474</v>
       </c>
-      <c r="T14" t="n">
+      <c r="U14" t="n">
         <v>0.151195750887588</v>
       </c>
-      <c r="U14" t="n">
+      <c r="V14" t="n">
         <v>-2.08441818950843</v>
       </c>
-      <c r="V14" t="n">
+      <c r="W14" t="n">
         <v>0.0388882596082964</v>
       </c>
     </row>
     <row r="15">
-      <c r="S15" t="n">
+      <c r="T15" t="n">
         <v>-0.723561957780729</v>
       </c>
-      <c r="T15" t="n">
+      <c r="U15" t="n">
         <v>0.240168942022631</v>
       </c>
-      <c r="U15" t="n">
+      <c r="V15" t="n">
         <v>-3.01272076100725</v>
       </c>
-      <c r="V15" t="n">
+      <c r="W15" t="n">
         <v>0.00305963409612887</v>
       </c>
     </row>
     <row r="16">
-      <c r="S16" t="n">
+      <c r="T16" t="n">
         <v>-1.02349781449083</v>
       </c>
-      <c r="T16" t="n">
+      <c r="U16" t="n">
         <v>0.333726298151483</v>
       </c>
-      <c r="U16" t="n">
+      <c r="V16" t="n">
         <v>-3.06687791810237</v>
       </c>
-      <c r="V16" t="n">
+      <c r="W16" t="n">
         <v>0.00258434378890403</v>
       </c>
     </row>
@@ -1777,7 +1777,7 @@
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AD18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1821,43 +1821,43 @@
       <c r="M19" t="s">
         <v>13</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AD19" t="s">
         <v>1</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AE19" t="s">
         <v>2</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AF19" t="s">
         <v>3</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AG19" t="s">
         <v>4</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AH19" t="s">
         <v>5</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AI19" t="s">
         <v>6</v>
       </c>
-      <c r="AH19" t="s">
+      <c r="AJ19" t="s">
         <v>7</v>
       </c>
-      <c r="AI19" t="s">
+      <c r="AK19" t="s">
         <v>8</v>
       </c>
-      <c r="AJ19" t="s">
+      <c r="AL19" t="s">
         <v>9</v>
       </c>
-      <c r="AK19" t="s">
+      <c r="AM19" t="s">
         <v>10</v>
       </c>
-      <c r="AL19" t="s">
+      <c r="AN19" t="s">
         <v>11</v>
       </c>
-      <c r="AM19" t="s">
+      <c r="AO19" t="s">
         <v>12</v>
       </c>
-      <c r="AN19" t="s">
+      <c r="AP19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1901,43 +1901,43 @@
       <c r="M20" t="n">
         <v>0.0676113162275986</v>
       </c>
-      <c r="AB20" t="n">
+      <c r="AD20" t="n">
         <v>1</v>
       </c>
-      <c r="AC20" t="n">
+      <c r="AE20" t="n">
         <v>150</v>
       </c>
-      <c r="AD20" t="n">
+      <c r="AF20" t="n">
         <v>5.84333333333333</v>
       </c>
-      <c r="AE20" t="n">
+      <c r="AG20" t="n">
         <v>0.828066127977863</v>
       </c>
-      <c r="AF20" t="n">
+      <c r="AH20" t="n">
         <v>5.8</v>
       </c>
-      <c r="AG20" t="n">
+      <c r="AI20" t="n">
         <v>5.80833333333333</v>
       </c>
-      <c r="AH20" t="n">
+      <c r="AJ20" t="n">
         <v>1.03782</v>
       </c>
-      <c r="AI20" t="n">
+      <c r="AK20" t="n">
         <v>4.3</v>
       </c>
-      <c r="AJ20" t="n">
+      <c r="AL20" t="n">
         <v>7.9</v>
       </c>
-      <c r="AK20" t="n">
+      <c r="AM20" t="n">
         <v>3.6</v>
       </c>
-      <c r="AL20" t="n">
+      <c r="AN20" t="n">
         <v>0.308640729589268</v>
       </c>
-      <c r="AM20" t="n">
+      <c r="AO20" t="n">
         <v>-0.60581253484815</v>
       </c>
-      <c r="AN20" t="n">
+      <c r="AP20" t="n">
         <v>0.0676113162275986</v>
       </c>
     </row>
@@ -1981,46 +1981,46 @@
       <c r="M21" t="n">
         <v>0.0355883331392484</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>25</v>
       </c>
-      <c r="AB21" t="n">
+      <c r="AD21" t="n">
         <v>2</v>
       </c>
-      <c r="AC21" t="n">
+      <c r="AE21" t="n">
         <v>150</v>
       </c>
-      <c r="AD21" t="n">
+      <c r="AF21" t="n">
         <v>3.05733333333333</v>
       </c>
-      <c r="AE21" t="n">
+      <c r="AG21" t="n">
         <v>0.435866284936698</v>
       </c>
-      <c r="AF21" t="n">
+      <c r="AH21" t="n">
         <v>3</v>
       </c>
-      <c r="AG21" t="n">
+      <c r="AI21" t="n">
         <v>3.04333333333333</v>
       </c>
-      <c r="AH21" t="n">
+      <c r="AJ21" t="n">
         <v>0.44478</v>
       </c>
-      <c r="AI21" t="n">
+      <c r="AK21" t="n">
         <v>2</v>
       </c>
-      <c r="AJ21" t="n">
+      <c r="AL21" t="n">
         <v>4.4</v>
       </c>
-      <c r="AK21" t="n">
+      <c r="AM21" t="n">
         <v>2.4</v>
       </c>
-      <c r="AL21" t="n">
+      <c r="AN21" t="n">
         <v>0.312614703922861</v>
       </c>
-      <c r="AM21" t="n">
+      <c r="AO21" t="n">
         <v>0.138704676680727</v>
       </c>
-      <c r="AN21" t="n">
+      <c r="AP21" t="n">
         <v>0.0355883331392484</v>
       </c>
     </row>
@@ -2064,49 +2064,49 @@
       <c r="M22" t="n">
         <v>0.144135997177411</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>17</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>18</v>
       </c>
-      <c r="AB22" t="n">
+      <c r="AD22" t="n">
         <v>3</v>
       </c>
-      <c r="AC22" t="n">
+      <c r="AE22" t="n">
         <v>150</v>
       </c>
-      <c r="AD22" t="n">
+      <c r="AF22" t="n">
         <v>3.758</v>
       </c>
-      <c r="AE22" t="n">
+      <c r="AG22" t="n">
         <v>1.76529823325947</v>
       </c>
-      <c r="AF22" t="n">
+      <c r="AH22" t="n">
         <v>4.35</v>
       </c>
-      <c r="AG22" t="n">
+      <c r="AI22" t="n">
         <v>3.76</v>
       </c>
-      <c r="AH22" t="n">
+      <c r="AJ22" t="n">
         <v>1.85325</v>
       </c>
-      <c r="AI22" t="n">
+      <c r="AK22" t="n">
         <v>1</v>
       </c>
-      <c r="AJ22" t="n">
+      <c r="AL22" t="n">
         <v>6.9</v>
       </c>
-      <c r="AK22" t="n">
+      <c r="AM22" t="n">
         <v>5.9</v>
       </c>
-      <c r="AL22" t="n">
+      <c r="AN22" t="n">
         <v>-0.269410930305303</v>
       </c>
-      <c r="AM22" t="n">
+      <c r="AO22" t="n">
         <v>-1.41685743173086</v>
       </c>
-      <c r="AN22" t="n">
+      <c r="AP22" t="n">
         <v>0.144135997177411</v>
       </c>
     </row>
@@ -2150,49 +2150,49 @@
       <c r="M23" t="n">
         <v>0.0622364450560443</v>
       </c>
-      <c r="S23" t="n">
+      <c r="T23" t="n">
         <v>4</v>
       </c>
-      <c r="T23" t="n">
+      <c r="U23" t="n">
         <v>2</v>
       </c>
-      <c r="AB23" t="n">
+      <c r="AD23" t="n">
         <v>4</v>
       </c>
-      <c r="AC23" t="n">
+      <c r="AE23" t="n">
         <v>150</v>
       </c>
-      <c r="AD23" t="n">
+      <c r="AF23" t="n">
         <v>1.19933333333333</v>
       </c>
-      <c r="AE23" t="n">
+      <c r="AG23" t="n">
         <v>0.762237668960347</v>
       </c>
-      <c r="AF23" t="n">
+      <c r="AH23" t="n">
         <v>1.3</v>
       </c>
-      <c r="AG23" t="n">
+      <c r="AI23" t="n">
         <v>1.18416666666667</v>
       </c>
-      <c r="AH23" t="n">
+      <c r="AJ23" t="n">
         <v>1.03782</v>
       </c>
-      <c r="AI23" t="n">
+      <c r="AK23" t="n">
         <v>0.1</v>
       </c>
-      <c r="AJ23" t="n">
+      <c r="AL23" t="n">
         <v>2.5</v>
       </c>
-      <c r="AK23" t="n">
+      <c r="AM23" t="n">
         <v>2.4</v>
       </c>
-      <c r="AL23" t="n">
+      <c r="AN23" t="n">
         <v>-0.100916565295792</v>
       </c>
-      <c r="AM23" t="n">
+      <c r="AO23" t="n">
         <v>-1.35817922060203</v>
       </c>
-      <c r="AN23" t="n">
+      <c r="AP23" t="n">
         <v>0.0622364450560443</v>
       </c>
     </row>
@@ -2236,49 +2236,49 @@
       <c r="M24" t="n">
         <v>0.0668900062090651</v>
       </c>
-      <c r="S24" t="n">
+      <c r="T24" t="n">
         <v>4</v>
       </c>
-      <c r="T24" t="n">
+      <c r="U24" t="n">
         <v>10</v>
       </c>
-      <c r="AB24" t="n">
+      <c r="AD24" t="n">
         <v>5</v>
       </c>
-      <c r="AC24" t="n">
+      <c r="AE24" t="n">
         <v>150</v>
-      </c>
-      <c r="AD24" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE24" t="n">
-        <v>0.81923192051904</v>
       </c>
       <c r="AF24" t="n">
         <v>2</v>
       </c>
       <c r="AG24" t="n">
+        <v>0.81923192051904</v>
+      </c>
+      <c r="AH24" t="n">
         <v>2</v>
       </c>
-      <c r="AH24" t="n">
+      <c r="AI24" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ24" t="n">
         <v>1.4826</v>
       </c>
-      <c r="AI24" t="n">
+      <c r="AK24" t="n">
         <v>1</v>
       </c>
-      <c r="AJ24" t="n">
+      <c r="AL24" t="n">
         <v>3</v>
       </c>
-      <c r="AK24" t="n">
+      <c r="AM24" t="n">
         <v>2</v>
       </c>
-      <c r="AL24" t="n">
+      <c r="AN24" t="n">
         <v>0</v>
       </c>
-      <c r="AM24" t="n">
+      <c r="AO24" t="n">
         <v>-1.51993333333333</v>
       </c>
-      <c r="AN24" t="n">
+      <c r="AP24" t="n">
         <v>0.0668900062090651</v>
       </c>
     </row>
@@ -2322,49 +2322,49 @@
       <c r="M25" t="n">
         <v>0.0676113162275986</v>
       </c>
-      <c r="S25" t="n">
+      <c r="T25" t="n">
         <v>7</v>
       </c>
-      <c r="T25" t="n">
+      <c r="U25" t="n">
         <v>4</v>
       </c>
-      <c r="AB25" t="n">
+      <c r="AD25" t="n">
         <v>1</v>
       </c>
-      <c r="AC25" t="n">
+      <c r="AE25" t="n">
         <v>150</v>
       </c>
-      <c r="AD25" t="n">
+      <c r="AF25" t="n">
         <v>5.84333333333333</v>
       </c>
-      <c r="AE25" t="n">
+      <c r="AG25" t="n">
         <v>0.828066127977863</v>
       </c>
-      <c r="AF25" t="n">
+      <c r="AH25" t="n">
         <v>5.8</v>
       </c>
-      <c r="AG25" t="n">
+      <c r="AI25" t="n">
         <v>5.80833333333333</v>
       </c>
-      <c r="AH25" t="n">
+      <c r="AJ25" t="n">
         <v>1.03782</v>
       </c>
-      <c r="AI25" t="n">
+      <c r="AK25" t="n">
         <v>4.3</v>
       </c>
-      <c r="AJ25" t="n">
+      <c r="AL25" t="n">
         <v>7.9</v>
       </c>
-      <c r="AK25" t="n">
+      <c r="AM25" t="n">
         <v>3.6</v>
       </c>
-      <c r="AL25" t="n">
+      <c r="AN25" t="n">
         <v>0.308640729589268</v>
       </c>
-      <c r="AM25" t="n">
+      <c r="AO25" t="n">
         <v>-0.60581253484815</v>
       </c>
-      <c r="AN25" t="n">
+      <c r="AP25" t="n">
         <v>0.0676113162275986</v>
       </c>
     </row>
@@ -2408,49 +2408,49 @@
       <c r="M26" t="n">
         <v>0.0355883331392484</v>
       </c>
-      <c r="S26" t="n">
+      <c r="T26" t="n">
         <v>7</v>
       </c>
-      <c r="T26" t="n">
+      <c r="U26" t="n">
         <v>22</v>
       </c>
-      <c r="AB26" t="n">
+      <c r="AD26" t="n">
         <v>2</v>
       </c>
-      <c r="AC26" t="n">
+      <c r="AE26" t="n">
         <v>150</v>
       </c>
-      <c r="AD26" t="n">
+      <c r="AF26" t="n">
         <v>3.05733333333333</v>
       </c>
-      <c r="AE26" t="n">
+      <c r="AG26" t="n">
         <v>0.435866284936698</v>
       </c>
-      <c r="AF26" t="n">
+      <c r="AH26" t="n">
         <v>3</v>
       </c>
-      <c r="AG26" t="n">
+      <c r="AI26" t="n">
         <v>3.04333333333333</v>
       </c>
-      <c r="AH26" t="n">
+      <c r="AJ26" t="n">
         <v>0.44478</v>
       </c>
-      <c r="AI26" t="n">
+      <c r="AK26" t="n">
         <v>2</v>
       </c>
-      <c r="AJ26" t="n">
+      <c r="AL26" t="n">
         <v>4.4</v>
       </c>
-      <c r="AK26" t="n">
+      <c r="AM26" t="n">
         <v>2.4</v>
       </c>
-      <c r="AL26" t="n">
+      <c r="AN26" t="n">
         <v>0.312614703922861</v>
       </c>
-      <c r="AM26" t="n">
+      <c r="AO26" t="n">
         <v>0.138704676680727</v>
       </c>
-      <c r="AN26" t="n">
+      <c r="AP26" t="n">
         <v>0.0355883331392484</v>
       </c>
     </row>
@@ -2494,49 +2494,49 @@
       <c r="M27" t="n">
         <v>0.144135997177411</v>
       </c>
-      <c r="S27" t="n">
+      <c r="T27" t="n">
         <v>8</v>
       </c>
-      <c r="T27" t="n">
+      <c r="U27" t="n">
         <v>16</v>
       </c>
-      <c r="AB27" t="n">
+      <c r="AD27" t="n">
         <v>3</v>
       </c>
-      <c r="AC27" t="n">
+      <c r="AE27" t="n">
         <v>150</v>
       </c>
-      <c r="AD27" t="n">
+      <c r="AF27" t="n">
         <v>3.758</v>
       </c>
-      <c r="AE27" t="n">
+      <c r="AG27" t="n">
         <v>1.76529823325947</v>
       </c>
-      <c r="AF27" t="n">
+      <c r="AH27" t="n">
         <v>4.35</v>
       </c>
-      <c r="AG27" t="n">
+      <c r="AI27" t="n">
         <v>3.76</v>
       </c>
-      <c r="AH27" t="n">
+      <c r="AJ27" t="n">
         <v>1.85325</v>
       </c>
-      <c r="AI27" t="n">
+      <c r="AK27" t="n">
         <v>1</v>
       </c>
-      <c r="AJ27" t="n">
+      <c r="AL27" t="n">
         <v>6.9</v>
       </c>
-      <c r="AK27" t="n">
+      <c r="AM27" t="n">
         <v>5.9</v>
       </c>
-      <c r="AL27" t="n">
+      <c r="AN27" t="n">
         <v>-0.269410930305303</v>
       </c>
-      <c r="AM27" t="n">
+      <c r="AO27" t="n">
         <v>-1.41685743173086</v>
       </c>
-      <c r="AN27" t="n">
+      <c r="AP27" t="n">
         <v>0.144135997177411</v>
       </c>
     </row>
@@ -2580,49 +2580,49 @@
       <c r="M28" t="n">
         <v>0.0622364450560443</v>
       </c>
-      <c r="S28" t="n">
+      <c r="T28" t="n">
         <v>9</v>
       </c>
-      <c r="T28" t="n">
+      <c r="U28" t="n">
         <v>10</v>
       </c>
-      <c r="AB28" t="n">
+      <c r="AD28" t="n">
         <v>4</v>
       </c>
-      <c r="AC28" t="n">
+      <c r="AE28" t="n">
         <v>150</v>
       </c>
-      <c r="AD28" t="n">
+      <c r="AF28" t="n">
         <v>1.19933333333333</v>
       </c>
-      <c r="AE28" t="n">
+      <c r="AG28" t="n">
         <v>0.762237668960347</v>
       </c>
-      <c r="AF28" t="n">
+      <c r="AH28" t="n">
         <v>1.3</v>
       </c>
-      <c r="AG28" t="n">
+      <c r="AI28" t="n">
         <v>1.18416666666667</v>
       </c>
-      <c r="AH28" t="n">
+      <c r="AJ28" t="n">
         <v>1.03782</v>
       </c>
-      <c r="AI28" t="n">
+      <c r="AK28" t="n">
         <v>0.1</v>
       </c>
-      <c r="AJ28" t="n">
+      <c r="AL28" t="n">
         <v>2.5</v>
       </c>
-      <c r="AK28" t="n">
+      <c r="AM28" t="n">
         <v>2.4</v>
       </c>
-      <c r="AL28" t="n">
+      <c r="AN28" t="n">
         <v>-0.100916565295792</v>
       </c>
-      <c r="AM28" t="n">
+      <c r="AO28" t="n">
         <v>-1.35817922060203</v>
       </c>
-      <c r="AN28" t="n">
+      <c r="AP28" t="n">
         <v>0.0622364450560443</v>
       </c>
     </row>
@@ -2666,81 +2666,81 @@
       <c r="M29" t="n">
         <v>0.0668900062090651</v>
       </c>
-      <c r="S29" t="n">
+      <c r="T29" t="n">
         <v>10</v>
       </c>
-      <c r="T29" t="n">
+      <c r="U29" t="n">
         <v>18</v>
       </c>
-      <c r="AB29" t="n">
+      <c r="AD29" t="n">
         <v>5</v>
       </c>
-      <c r="AC29" t="n">
+      <c r="AE29" t="n">
         <v>150</v>
-      </c>
-      <c r="AD29" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE29" t="n">
-        <v>0.81923192051904</v>
       </c>
       <c r="AF29" t="n">
         <v>2</v>
       </c>
       <c r="AG29" t="n">
+        <v>0.81923192051904</v>
+      </c>
+      <c r="AH29" t="n">
         <v>2</v>
       </c>
-      <c r="AH29" t="n">
+      <c r="AI29" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ29" t="n">
         <v>1.4826</v>
       </c>
-      <c r="AI29" t="n">
+      <c r="AK29" t="n">
         <v>1</v>
       </c>
-      <c r="AJ29" t="n">
+      <c r="AL29" t="n">
         <v>3</v>
       </c>
-      <c r="AK29" t="n">
+      <c r="AM29" t="n">
         <v>2</v>
       </c>
-      <c r="AL29" t="n">
+      <c r="AN29" t="n">
         <v>0</v>
       </c>
-      <c r="AM29" t="n">
+      <c r="AO29" t="n">
         <v>-1.51993333333333</v>
       </c>
-      <c r="AN29" t="n">
+      <c r="AP29" t="n">
         <v>0.0668900062090651</v>
       </c>
     </row>
     <row r="30">
-      <c r="S30" t="n">
+      <c r="T30" t="n">
         <v>10</v>
       </c>
-      <c r="T30" t="n">
+      <c r="U30" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="31">
-      <c r="S31" t="n">
+      <c r="T31" t="n">
         <v>10</v>
       </c>
-      <c r="T31" t="n">
+      <c r="U31" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="32">
-      <c r="S32" t="n">
+      <c r="T32" t="n">
         <v>11</v>
       </c>
-      <c r="T32" t="n">
+      <c r="U32" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="33">
-      <c r="S33" t="n">
+      <c r="T33" t="n">
         <v>11</v>
       </c>
-      <c r="T33" t="n">
+      <c r="U33" t="n">
         <v>28</v>
       </c>
     </row>
@@ -2748,205 +2748,205 @@
       <c r="A34" t="s">
         <v>15</v>
       </c>
-      <c r="S34" t="n">
+      <c r="T34" t="n">
         <v>12</v>
       </c>
-      <c r="T34" t="n">
+      <c r="U34" t="n">
         <v>14</v>
       </c>
-      <c r="AB34" t="s">
+      <c r="AD34" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="35">
-      <c r="S35" t="n">
+      <c r="T35" t="n">
         <v>12</v>
       </c>
-      <c r="T35" t="n">
+      <c r="U35" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="36">
-      <c r="S36" t="n">
+      <c r="T36" t="n">
         <v>12</v>
       </c>
-      <c r="T36" t="n">
+      <c r="U36" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="37">
-      <c r="S37" t="n">
+      <c r="T37" t="n">
         <v>12</v>
       </c>
-      <c r="T37" t="n">
+      <c r="U37" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="38">
-      <c r="S38" t="n">
+      <c r="T38" t="n">
         <v>13</v>
       </c>
-      <c r="T38" t="n">
+      <c r="U38" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="39">
-      <c r="S39" t="n">
+      <c r="T39" t="n">
         <v>13</v>
       </c>
-      <c r="T39" t="n">
+      <c r="U39" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="40">
-      <c r="S40" t="n">
+      <c r="T40" t="n">
         <v>13</v>
       </c>
-      <c r="T40" t="n">
+      <c r="U40" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="41">
-      <c r="S41" t="n">
+      <c r="T41" t="n">
         <v>13</v>
       </c>
-      <c r="T41" t="n">
+      <c r="U41" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="42">
-      <c r="S42" t="n">
+      <c r="T42" t="n">
         <v>14</v>
       </c>
-      <c r="T42" t="n">
+      <c r="U42" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="43">
-      <c r="S43" t="n">
+      <c r="T43" t="n">
         <v>14</v>
       </c>
-      <c r="T43" t="n">
+      <c r="U43" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="44">
-      <c r="S44" t="n">
+      <c r="T44" t="n">
         <v>14</v>
       </c>
-      <c r="T44" t="n">
+      <c r="U44" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="45">
-      <c r="S45" t="n">
+      <c r="T45" t="n">
         <v>14</v>
       </c>
-      <c r="T45" t="n">
+      <c r="U45" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="46">
-      <c r="S46" t="n">
+      <c r="T46" t="n">
         <v>15</v>
       </c>
-      <c r="T46" t="n">
+      <c r="U46" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="47">
-      <c r="S47" t="n">
+      <c r="T47" t="n">
         <v>15</v>
       </c>
-      <c r="T47" t="n">
+      <c r="U47" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="48">
-      <c r="S48" t="n">
+      <c r="T48" t="n">
         <v>15</v>
       </c>
-      <c r="T48" t="n">
+      <c r="U48" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="49">
-      <c r="S49" t="n">
+      <c r="T49" t="n">
         <v>16</v>
       </c>
-      <c r="T49" t="n">
+      <c r="U49" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="50">
-      <c r="S50" t="n">
+      <c r="T50" t="n">
         <v>16</v>
       </c>
-      <c r="T50" t="n">
+      <c r="U50" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="51">
-      <c r="S51" t="n">
+      <c r="T51" t="n">
         <v>17</v>
       </c>
-      <c r="T51" t="n">
+      <c r="U51" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="52">
-      <c r="S52" t="n">
+      <c r="T52" t="n">
         <v>17</v>
       </c>
-      <c r="T52" t="n">
+      <c r="U52" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="53">
-      <c r="S53" t="n">
+      <c r="T53" t="n">
         <v>17</v>
       </c>
-      <c r="T53" t="n">
+      <c r="U53" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="54">
-      <c r="S54" t="n">
+      <c r="T54" t="n">
         <v>18</v>
       </c>
-      <c r="T54" t="n">
+      <c r="U54" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="55">
-      <c r="S55" t="n">
+      <c r="T55" t="n">
         <v>18</v>
       </c>
-      <c r="T55" t="n">
+      <c r="U55" t="n">
         <v>56</v>
       </c>
     </row>
     <row r="56">
-      <c r="S56" t="n">
+      <c r="T56" t="n">
         <v>18</v>
       </c>
-      <c r="T56" t="n">
+      <c r="U56" t="n">
         <v>76</v>
       </c>
     </row>
     <row r="57">
-      <c r="S57" t="n">
+      <c r="T57" t="n">
         <v>18</v>
       </c>
-      <c r="T57" t="n">
+      <c r="U57" t="n">
         <v>84</v>
       </c>
     </row>
     <row r="58">
-      <c r="S58" t="n">
+      <c r="T58" t="n">
         <v>19</v>
       </c>
-      <c r="T58" t="n">
+      <c r="U58" t="n">
         <v>36</v>
       </c>
     </row>
@@ -2954,13 +2954,13 @@
       <c r="A59" t="s">
         <v>16</v>
       </c>
-      <c r="S59" t="n">
+      <c r="T59" t="n">
         <v>19</v>
       </c>
-      <c r="T59" t="n">
+      <c r="U59" t="n">
         <v>46</v>
       </c>
-      <c r="AB59" t="s">
+      <c r="AD59" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2971,16 +2971,16 @@
       <c r="B60" t="s">
         <v>18</v>
       </c>
-      <c r="S60" t="n">
+      <c r="T60" t="n">
         <v>19</v>
       </c>
-      <c r="T60" t="n">
+      <c r="U60" t="n">
         <v>68</v>
       </c>
-      <c r="AB60" t="s">
+      <c r="AD60" t="s">
         <v>17</v>
       </c>
-      <c r="AC60" t="s">
+      <c r="AE60" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2991,16 +2991,16 @@
       <c r="B61" t="n">
         <v>2</v>
       </c>
-      <c r="S61" t="n">
+      <c r="T61" t="n">
         <v>20</v>
       </c>
-      <c r="T61" t="n">
+      <c r="U61" t="n">
         <v>32</v>
       </c>
-      <c r="AB61" t="n">
+      <c r="AD61" t="n">
         <v>4</v>
       </c>
-      <c r="AC61" t="n">
+      <c r="AE61" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3011,16 +3011,16 @@
       <c r="B62" t="n">
         <v>10</v>
       </c>
-      <c r="S62" t="n">
+      <c r="T62" t="n">
         <v>20</v>
       </c>
-      <c r="T62" t="n">
+      <c r="U62" t="n">
         <v>48</v>
       </c>
-      <c r="AB62" t="n">
+      <c r="AD62" t="n">
         <v>4</v>
       </c>
-      <c r="AC62" t="n">
+      <c r="AE62" t="n">
         <v>10</v>
       </c>
     </row>
@@ -3031,16 +3031,16 @@
       <c r="B63" t="n">
         <v>4</v>
       </c>
-      <c r="S63" t="n">
+      <c r="T63" t="n">
         <v>20</v>
       </c>
-      <c r="T63" t="n">
+      <c r="U63" t="n">
         <v>52</v>
       </c>
-      <c r="AB63" t="n">
+      <c r="AD63" t="n">
         <v>7</v>
       </c>
-      <c r="AC63" t="n">
+      <c r="AE63" t="n">
         <v>4</v>
       </c>
     </row>
@@ -3051,16 +3051,16 @@
       <c r="B64" t="n">
         <v>22</v>
       </c>
-      <c r="S64" t="n">
+      <c r="T64" t="n">
         <v>20</v>
       </c>
-      <c r="T64" t="n">
+      <c r="U64" t="n">
         <v>56</v>
       </c>
-      <c r="AB64" t="n">
+      <c r="AD64" t="n">
         <v>7</v>
       </c>
-      <c r="AC64" t="n">
+      <c r="AE64" t="n">
         <v>22</v>
       </c>
     </row>
@@ -3071,16 +3071,16 @@
       <c r="B65" t="n">
         <v>16</v>
       </c>
-      <c r="S65" t="n">
+      <c r="T65" t="n">
         <v>20</v>
       </c>
-      <c r="T65" t="n">
+      <c r="U65" t="n">
         <v>64</v>
       </c>
-      <c r="AB65" t="n">
+      <c r="AD65" t="n">
         <v>8</v>
       </c>
-      <c r="AC65" t="n">
+      <c r="AE65" t="n">
         <v>16</v>
       </c>
     </row>
@@ -3091,16 +3091,16 @@
       <c r="B66" t="n">
         <v>10</v>
       </c>
-      <c r="S66" t="n">
+      <c r="T66" t="n">
         <v>22</v>
       </c>
-      <c r="T66" t="n">
+      <c r="U66" t="n">
         <v>66</v>
       </c>
-      <c r="AB66" t="n">
+      <c r="AD66" t="n">
         <v>9</v>
       </c>
-      <c r="AC66" t="n">
+      <c r="AE66" t="n">
         <v>10</v>
       </c>
     </row>
@@ -3111,16 +3111,16 @@
       <c r="B67" t="n">
         <v>18</v>
       </c>
-      <c r="S67" t="n">
+      <c r="T67" t="n">
         <v>23</v>
       </c>
-      <c r="T67" t="n">
+      <c r="U67" t="n">
         <v>54</v>
       </c>
-      <c r="AB67" t="n">
+      <c r="AD67" t="n">
         <v>10</v>
       </c>
-      <c r="AC67" t="n">
+      <c r="AE67" t="n">
         <v>18</v>
       </c>
     </row>
@@ -3131,16 +3131,16 @@
       <c r="B68" t="n">
         <v>26</v>
       </c>
-      <c r="S68" t="n">
+      <c r="T68" t="n">
         <v>24</v>
       </c>
-      <c r="T68" t="n">
+      <c r="U68" t="n">
         <v>70</v>
       </c>
-      <c r="AB68" t="n">
+      <c r="AD68" t="n">
         <v>10</v>
       </c>
-      <c r="AC68" t="n">
+      <c r="AE68" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3151,16 +3151,16 @@
       <c r="B69" t="n">
         <v>34</v>
       </c>
-      <c r="S69" t="n">
+      <c r="T69" t="n">
         <v>24</v>
       </c>
-      <c r="T69" t="n">
+      <c r="U69" t="n">
         <v>92</v>
       </c>
-      <c r="AB69" t="n">
+      <c r="AD69" t="n">
         <v>10</v>
       </c>
-      <c r="AC69" t="n">
+      <c r="AE69" t="n">
         <v>34</v>
       </c>
     </row>
@@ -3171,16 +3171,16 @@
       <c r="B70" t="n">
         <v>17</v>
       </c>
-      <c r="S70" t="n">
+      <c r="T70" t="n">
         <v>24</v>
       </c>
-      <c r="T70" t="n">
+      <c r="U70" t="n">
         <v>93</v>
       </c>
-      <c r="AB70" t="n">
+      <c r="AD70" t="n">
         <v>11</v>
       </c>
-      <c r="AC70" t="n">
+      <c r="AE70" t="n">
         <v>17</v>
       </c>
     </row>
@@ -3191,16 +3191,16 @@
       <c r="B71" t="n">
         <v>28</v>
       </c>
-      <c r="S71" t="n">
+      <c r="T71" t="n">
         <v>24</v>
       </c>
-      <c r="T71" t="n">
+      <c r="U71" t="n">
         <v>120</v>
       </c>
-      <c r="AB71" t="n">
+      <c r="AD71" t="n">
         <v>11</v>
       </c>
-      <c r="AC71" t="n">
+      <c r="AE71" t="n">
         <v>28</v>
       </c>
     </row>
@@ -3211,16 +3211,16 @@
       <c r="B72" t="n">
         <v>14</v>
       </c>
-      <c r="S72" t="n">
+      <c r="T72" t="n">
         <v>25</v>
       </c>
-      <c r="T72" t="n">
+      <c r="U72" t="n">
         <v>85</v>
       </c>
-      <c r="AB72" t="n">
+      <c r="AD72" t="n">
         <v>12</v>
       </c>
-      <c r="AC72" t="n">
+      <c r="AE72" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3231,10 +3231,10 @@
       <c r="B73" t="n">
         <v>20</v>
       </c>
-      <c r="AB73" t="n">
+      <c r="AD73" t="n">
         <v>12</v>
       </c>
-      <c r="AC73" t="n">
+      <c r="AE73" t="n">
         <v>20</v>
       </c>
     </row>
@@ -3245,10 +3245,10 @@
       <c r="B74" t="n">
         <v>24</v>
       </c>
-      <c r="AB74" t="n">
+      <c r="AD74" t="n">
         <v>12</v>
       </c>
-      <c r="AC74" t="n">
+      <c r="AE74" t="n">
         <v>24</v>
       </c>
     </row>
@@ -3259,10 +3259,10 @@
       <c r="B75" t="n">
         <v>28</v>
       </c>
-      <c r="AB75" t="n">
+      <c r="AD75" t="n">
         <v>12</v>
       </c>
-      <c r="AC75" t="n">
+      <c r="AE75" t="n">
         <v>28</v>
       </c>
     </row>
@@ -3273,10 +3273,10 @@
       <c r="B76" t="n">
         <v>26</v>
       </c>
-      <c r="AB76" t="n">
+      <c r="AD76" t="n">
         <v>13</v>
       </c>
-      <c r="AC76" t="n">
+      <c r="AE76" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3287,13 +3287,13 @@
       <c r="B77" t="n">
         <v>34</v>
       </c>
-      <c r="S77" t="s">
+      <c r="T77" t="s">
         <v>26</v>
       </c>
-      <c r="AB77" t="n">
+      <c r="AD77" t="n">
         <v>13</v>
       </c>
-      <c r="AC77" t="n">
+      <c r="AE77" t="n">
         <v>34</v>
       </c>
     </row>
@@ -3304,16 +3304,16 @@
       <c r="B78" t="n">
         <v>34</v>
       </c>
-      <c r="S78" t="s">
+      <c r="T78" t="s">
         <v>17</v>
       </c>
-      <c r="T78" t="s">
+      <c r="U78" t="s">
         <v>18</v>
       </c>
-      <c r="AB78" t="n">
+      <c r="AD78" t="n">
         <v>13</v>
       </c>
-      <c r="AC78" t="n">
+      <c r="AE78" t="n">
         <v>34</v>
       </c>
     </row>
@@ -3324,16 +3324,16 @@
       <c r="B79" t="n">
         <v>46</v>
       </c>
-      <c r="S79" t="n">
+      <c r="T79" t="n">
         <v>4</v>
       </c>
-      <c r="T79" t="n">
+      <c r="U79" t="n">
         <v>2</v>
       </c>
-      <c r="AB79" t="n">
+      <c r="AD79" t="n">
         <v>13</v>
       </c>
-      <c r="AC79" t="n">
+      <c r="AE79" t="n">
         <v>46</v>
       </c>
     </row>
@@ -3344,16 +3344,16 @@
       <c r="B80" t="n">
         <v>26</v>
       </c>
-      <c r="S80" t="n">
+      <c r="T80" t="n">
         <v>4</v>
       </c>
-      <c r="T80" t="n">
+      <c r="U80" t="n">
         <v>10</v>
       </c>
-      <c r="AB80" t="n">
+      <c r="AD80" t="n">
         <v>14</v>
       </c>
-      <c r="AC80" t="n">
+      <c r="AE80" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3364,16 +3364,16 @@
       <c r="B81" t="n">
         <v>36</v>
       </c>
-      <c r="S81" t="n">
+      <c r="T81" t="n">
         <v>7</v>
       </c>
-      <c r="T81" t="n">
+      <c r="U81" t="n">
         <v>4</v>
       </c>
-      <c r="AB81" t="n">
+      <c r="AD81" t="n">
         <v>14</v>
       </c>
-      <c r="AC81" t="n">
+      <c r="AE81" t="n">
         <v>36</v>
       </c>
     </row>
@@ -3384,16 +3384,16 @@
       <c r="B82" t="n">
         <v>60</v>
       </c>
-      <c r="S82" t="n">
+      <c r="T82" t="n">
         <v>7</v>
       </c>
-      <c r="T82" t="n">
+      <c r="U82" t="n">
         <v>22</v>
       </c>
-      <c r="AB82" t="n">
+      <c r="AD82" t="n">
         <v>14</v>
       </c>
-      <c r="AC82" t="n">
+      <c r="AE82" t="n">
         <v>60</v>
       </c>
     </row>
@@ -3404,16 +3404,16 @@
       <c r="B83" t="n">
         <v>80</v>
       </c>
-      <c r="S83" t="n">
+      <c r="T83" t="n">
         <v>8</v>
       </c>
-      <c r="T83" t="n">
+      <c r="U83" t="n">
         <v>16</v>
       </c>
-      <c r="AB83" t="n">
+      <c r="AD83" t="n">
         <v>14</v>
       </c>
-      <c r="AC83" t="n">
+      <c r="AE83" t="n">
         <v>80</v>
       </c>
     </row>
@@ -3424,16 +3424,16 @@
       <c r="B84" t="n">
         <v>20</v>
       </c>
-      <c r="S84" t="n">
+      <c r="T84" t="n">
         <v>9</v>
       </c>
-      <c r="T84" t="n">
+      <c r="U84" t="n">
         <v>10</v>
       </c>
-      <c r="AB84" t="n">
+      <c r="AD84" t="n">
         <v>15</v>
       </c>
-      <c r="AC84" t="n">
+      <c r="AE84" t="n">
         <v>20</v>
       </c>
     </row>
@@ -3444,16 +3444,16 @@
       <c r="B85" t="n">
         <v>26</v>
       </c>
-      <c r="S85" t="n">
+      <c r="T85" t="n">
         <v>10</v>
       </c>
-      <c r="T85" t="n">
+      <c r="U85" t="n">
         <v>18</v>
       </c>
-      <c r="AB85" t="n">
+      <c r="AD85" t="n">
         <v>15</v>
       </c>
-      <c r="AC85" t="n">
+      <c r="AE85" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3464,16 +3464,16 @@
       <c r="B86" t="n">
         <v>54</v>
       </c>
-      <c r="S86" t="n">
+      <c r="T86" t="n">
         <v>10</v>
       </c>
-      <c r="T86" t="n">
+      <c r="U86" t="n">
         <v>26</v>
       </c>
-      <c r="AB86" t="n">
+      <c r="AD86" t="n">
         <v>15</v>
       </c>
-      <c r="AC86" t="n">
+      <c r="AE86" t="n">
         <v>54</v>
       </c>
     </row>
@@ -3484,16 +3484,16 @@
       <c r="B87" t="n">
         <v>32</v>
       </c>
-      <c r="S87" t="n">
+      <c r="T87" t="n">
         <v>10</v>
       </c>
-      <c r="T87" t="n">
+      <c r="U87" t="n">
         <v>34</v>
       </c>
-      <c r="AB87" t="n">
+      <c r="AD87" t="n">
         <v>16</v>
       </c>
-      <c r="AC87" t="n">
+      <c r="AE87" t="n">
         <v>32</v>
       </c>
     </row>
@@ -3504,16 +3504,16 @@
       <c r="B88" t="n">
         <v>40</v>
       </c>
-      <c r="S88" t="n">
+      <c r="T88" t="n">
         <v>11</v>
       </c>
-      <c r="T88" t="n">
+      <c r="U88" t="n">
         <v>17</v>
       </c>
-      <c r="AB88" t="n">
+      <c r="AD88" t="n">
         <v>16</v>
       </c>
-      <c r="AC88" t="n">
+      <c r="AE88" t="n">
         <v>40</v>
       </c>
     </row>
@@ -3524,16 +3524,16 @@
       <c r="B89" t="n">
         <v>32</v>
       </c>
-      <c r="S89" t="n">
+      <c r="T89" t="n">
         <v>11</v>
       </c>
-      <c r="T89" t="n">
+      <c r="U89" t="n">
         <v>28</v>
       </c>
-      <c r="AB89" t="n">
+      <c r="AD89" t="n">
         <v>17</v>
       </c>
-      <c r="AC89" t="n">
+      <c r="AE89" t="n">
         <v>32</v>
       </c>
     </row>
@@ -3544,16 +3544,16 @@
       <c r="B90" t="n">
         <v>40</v>
       </c>
-      <c r="S90" t="n">
+      <c r="T90" t="n">
         <v>12</v>
       </c>
-      <c r="T90" t="n">
+      <c r="U90" t="n">
         <v>14</v>
       </c>
-      <c r="AB90" t="n">
+      <c r="AD90" t="n">
         <v>17</v>
       </c>
-      <c r="AC90" t="n">
+      <c r="AE90" t="n">
         <v>40</v>
       </c>
     </row>
@@ -3564,16 +3564,16 @@
       <c r="B91" t="n">
         <v>50</v>
       </c>
-      <c r="S91" t="n">
+      <c r="T91" t="n">
         <v>12</v>
       </c>
-      <c r="T91" t="n">
+      <c r="U91" t="n">
         <v>20</v>
       </c>
-      <c r="AB91" t="n">
+      <c r="AD91" t="n">
         <v>17</v>
       </c>
-      <c r="AC91" t="n">
+      <c r="AE91" t="n">
         <v>50</v>
       </c>
     </row>
@@ -3584,16 +3584,16 @@
       <c r="B92" t="n">
         <v>42</v>
       </c>
-      <c r="S92" t="n">
+      <c r="T92" t="n">
         <v>12</v>
       </c>
-      <c r="T92" t="n">
+      <c r="U92" t="n">
         <v>24</v>
       </c>
-      <c r="AB92" t="n">
+      <c r="AD92" t="n">
         <v>18</v>
       </c>
-      <c r="AC92" t="n">
+      <c r="AE92" t="n">
         <v>42</v>
       </c>
     </row>
@@ -3604,16 +3604,16 @@
       <c r="B93" t="n">
         <v>56</v>
       </c>
-      <c r="S93" t="n">
+      <c r="T93" t="n">
         <v>12</v>
       </c>
-      <c r="T93" t="n">
+      <c r="U93" t="n">
         <v>28</v>
       </c>
-      <c r="AB93" t="n">
+      <c r="AD93" t="n">
         <v>18</v>
       </c>
-      <c r="AC93" t="n">
+      <c r="AE93" t="n">
         <v>56</v>
       </c>
     </row>
@@ -3624,16 +3624,16 @@
       <c r="B94" t="n">
         <v>76</v>
       </c>
-      <c r="S94" t="n">
+      <c r="T94" t="n">
         <v>13</v>
       </c>
-      <c r="T94" t="n">
+      <c r="U94" t="n">
         <v>26</v>
       </c>
-      <c r="AB94" t="n">
+      <c r="AD94" t="n">
         <v>18</v>
       </c>
-      <c r="AC94" t="n">
+      <c r="AE94" t="n">
         <v>76</v>
       </c>
     </row>
@@ -3644,16 +3644,16 @@
       <c r="B95" t="n">
         <v>84</v>
       </c>
-      <c r="S95" t="n">
+      <c r="T95" t="n">
         <v>13</v>
       </c>
-      <c r="T95" t="n">
+      <c r="U95" t="n">
         <v>34</v>
       </c>
-      <c r="AB95" t="n">
+      <c r="AD95" t="n">
         <v>18</v>
       </c>
-      <c r="AC95" t="n">
+      <c r="AE95" t="n">
         <v>84</v>
       </c>
     </row>
@@ -3664,16 +3664,16 @@
       <c r="B96" t="n">
         <v>36</v>
       </c>
-      <c r="S96" t="n">
+      <c r="T96" t="n">
         <v>13</v>
       </c>
-      <c r="T96" t="n">
+      <c r="U96" t="n">
         <v>34</v>
       </c>
-      <c r="AB96" t="n">
+      <c r="AD96" t="n">
         <v>19</v>
       </c>
-      <c r="AC96" t="n">
+      <c r="AE96" t="n">
         <v>36</v>
       </c>
     </row>
@@ -3684,16 +3684,16 @@
       <c r="B97" t="n">
         <v>46</v>
       </c>
-      <c r="S97" t="n">
+      <c r="T97" t="n">
         <v>13</v>
       </c>
-      <c r="T97" t="n">
+      <c r="U97" t="n">
         <v>46</v>
       </c>
-      <c r="AB97" t="n">
+      <c r="AD97" t="n">
         <v>19</v>
       </c>
-      <c r="AC97" t="n">
+      <c r="AE97" t="n">
         <v>46</v>
       </c>
     </row>
@@ -3704,16 +3704,16 @@
       <c r="B98" t="n">
         <v>68</v>
       </c>
-      <c r="S98" t="n">
+      <c r="T98" t="n">
         <v>14</v>
       </c>
-      <c r="T98" t="n">
+      <c r="U98" t="n">
         <v>26</v>
       </c>
-      <c r="AB98" t="n">
+      <c r="AD98" t="n">
         <v>19</v>
       </c>
-      <c r="AC98" t="n">
+      <c r="AE98" t="n">
         <v>68</v>
       </c>
     </row>
@@ -3724,16 +3724,16 @@
       <c r="B99" t="n">
         <v>32</v>
       </c>
-      <c r="S99" t="n">
+      <c r="T99" t="n">
         <v>14</v>
       </c>
-      <c r="T99" t="n">
+      <c r="U99" t="n">
         <v>36</v>
       </c>
-      <c r="AB99" t="n">
+      <c r="AD99" t="n">
         <v>20</v>
       </c>
-      <c r="AC99" t="n">
+      <c r="AE99" t="n">
         <v>32</v>
       </c>
     </row>
@@ -3744,16 +3744,16 @@
       <c r="B100" t="n">
         <v>48</v>
       </c>
-      <c r="S100" t="n">
+      <c r="T100" t="n">
         <v>14</v>
       </c>
-      <c r="T100" t="n">
+      <c r="U100" t="n">
         <v>60</v>
       </c>
-      <c r="AB100" t="n">
+      <c r="AD100" t="n">
         <v>20</v>
       </c>
-      <c r="AC100" t="n">
+      <c r="AE100" t="n">
         <v>48</v>
       </c>
     </row>
@@ -3764,16 +3764,16 @@
       <c r="B101" t="n">
         <v>52</v>
       </c>
-      <c r="S101" t="n">
+      <c r="T101" t="n">
         <v>14</v>
       </c>
-      <c r="T101" t="n">
+      <c r="U101" t="n">
         <v>80</v>
       </c>
-      <c r="AB101" t="n">
+      <c r="AD101" t="n">
         <v>20</v>
       </c>
-      <c r="AC101" t="n">
+      <c r="AE101" t="n">
         <v>52</v>
       </c>
     </row>
@@ -3784,16 +3784,16 @@
       <c r="B102" t="n">
         <v>56</v>
       </c>
-      <c r="S102" t="n">
+      <c r="T102" t="n">
         <v>15</v>
       </c>
-      <c r="T102" t="n">
+      <c r="U102" t="n">
         <v>20</v>
       </c>
-      <c r="AB102" t="n">
+      <c r="AD102" t="n">
         <v>20</v>
       </c>
-      <c r="AC102" t="n">
+      <c r="AE102" t="n">
         <v>56</v>
       </c>
     </row>
@@ -3804,16 +3804,16 @@
       <c r="B103" t="n">
         <v>64</v>
       </c>
-      <c r="S103" t="n">
+      <c r="T103" t="n">
         <v>15</v>
       </c>
-      <c r="T103" t="n">
+      <c r="U103" t="n">
         <v>26</v>
       </c>
-      <c r="AB103" t="n">
+      <c r="AD103" t="n">
         <v>20</v>
       </c>
-      <c r="AC103" t="n">
+      <c r="AE103" t="n">
         <v>64</v>
       </c>
     </row>
@@ -3824,16 +3824,16 @@
       <c r="B104" t="n">
         <v>66</v>
       </c>
-      <c r="S104" t="n">
+      <c r="T104" t="n">
         <v>15</v>
       </c>
-      <c r="T104" t="n">
+      <c r="U104" t="n">
         <v>54</v>
       </c>
-      <c r="AB104" t="n">
+      <c r="AD104" t="n">
         <v>22</v>
       </c>
-      <c r="AC104" t="n">
+      <c r="AE104" t="n">
         <v>66</v>
       </c>
     </row>
@@ -3844,16 +3844,16 @@
       <c r="B105" t="n">
         <v>54</v>
       </c>
-      <c r="S105" t="n">
+      <c r="T105" t="n">
         <v>16</v>
       </c>
-      <c r="T105" t="n">
+      <c r="U105" t="n">
         <v>32</v>
       </c>
-      <c r="AB105" t="n">
+      <c r="AD105" t="n">
         <v>23</v>
       </c>
-      <c r="AC105" t="n">
+      <c r="AE105" t="n">
         <v>54</v>
       </c>
     </row>
@@ -3864,16 +3864,16 @@
       <c r="B106" t="n">
         <v>70</v>
       </c>
-      <c r="S106" t="n">
+      <c r="T106" t="n">
         <v>16</v>
       </c>
-      <c r="T106" t="n">
+      <c r="U106" t="n">
         <v>40</v>
       </c>
-      <c r="AB106" t="n">
+      <c r="AD106" t="n">
         <v>24</v>
       </c>
-      <c r="AC106" t="n">
+      <c r="AE106" t="n">
         <v>70</v>
       </c>
     </row>
@@ -3884,16 +3884,16 @@
       <c r="B107" t="n">
         <v>92</v>
       </c>
-      <c r="S107" t="n">
+      <c r="T107" t="n">
         <v>17</v>
       </c>
-      <c r="T107" t="n">
+      <c r="U107" t="n">
         <v>32</v>
       </c>
-      <c r="AB107" t="n">
+      <c r="AD107" t="n">
         <v>24</v>
       </c>
-      <c r="AC107" t="n">
+      <c r="AE107" t="n">
         <v>92</v>
       </c>
     </row>
@@ -3904,16 +3904,16 @@
       <c r="B108" t="n">
         <v>93</v>
       </c>
-      <c r="S108" t="n">
+      <c r="T108" t="n">
         <v>17</v>
       </c>
-      <c r="T108" t="n">
+      <c r="U108" t="n">
         <v>40</v>
       </c>
-      <c r="AB108" t="n">
+      <c r="AD108" t="n">
         <v>24</v>
       </c>
-      <c r="AC108" t="n">
+      <c r="AE108" t="n">
         <v>93</v>
       </c>
     </row>
@@ -3924,16 +3924,16 @@
       <c r="B109" t="n">
         <v>120</v>
       </c>
-      <c r="S109" t="n">
+      <c r="T109" t="n">
         <v>17</v>
       </c>
-      <c r="T109" t="n">
+      <c r="U109" t="n">
         <v>50</v>
       </c>
-      <c r="AB109" t="n">
+      <c r="AD109" t="n">
         <v>24</v>
       </c>
-      <c r="AC109" t="n">
+      <c r="AE109" t="n">
         <v>120</v>
       </c>
     </row>
@@ -3944,573 +3944,573 @@
       <c r="B110" t="n">
         <v>85</v>
       </c>
-      <c r="S110" t="n">
+      <c r="T110" t="n">
         <v>18</v>
       </c>
-      <c r="T110" t="n">
+      <c r="U110" t="n">
         <v>42</v>
       </c>
-      <c r="AB110" t="n">
+      <c r="AD110" t="n">
         <v>25</v>
       </c>
-      <c r="AC110" t="n">
+      <c r="AE110" t="n">
         <v>85</v>
       </c>
     </row>
     <row r="111">
-      <c r="S111" t="n">
+      <c r="T111" t="n">
         <v>18</v>
       </c>
-      <c r="T111" t="n">
+      <c r="U111" t="n">
         <v>56</v>
       </c>
     </row>
     <row r="112">
-      <c r="S112" t="n">
+      <c r="T112" t="n">
         <v>18</v>
       </c>
-      <c r="T112" t="n">
+      <c r="U112" t="n">
         <v>76</v>
       </c>
     </row>
     <row r="113">
-      <c r="S113" t="n">
+      <c r="T113" t="n">
         <v>18</v>
       </c>
-      <c r="T113" t="n">
+      <c r="U113" t="n">
         <v>84</v>
       </c>
     </row>
     <row r="114">
-      <c r="S114" t="n">
+      <c r="T114" t="n">
         <v>19</v>
       </c>
-      <c r="T114" t="n">
+      <c r="U114" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="115">
-      <c r="S115" t="n">
+      <c r="T115" t="n">
         <v>19</v>
       </c>
-      <c r="T115" t="n">
+      <c r="U115" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="116">
-      <c r="S116" t="n">
+      <c r="T116" t="n">
         <v>19</v>
       </c>
-      <c r="T116" t="n">
+      <c r="U116" t="n">
         <v>68</v>
       </c>
     </row>
     <row r="117">
-      <c r="S117" t="n">
+      <c r="T117" t="n">
         <v>20</v>
       </c>
-      <c r="T117" t="n">
+      <c r="U117" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="118">
-      <c r="S118" t="n">
+      <c r="T118" t="n">
         <v>20</v>
       </c>
-      <c r="T118" t="n">
+      <c r="U118" t="n">
         <v>48</v>
       </c>
     </row>
     <row r="119">
-      <c r="S119" t="n">
+      <c r="T119" t="n">
         <v>20</v>
       </c>
-      <c r="T119" t="n">
+      <c r="U119" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="120">
-      <c r="S120" t="n">
+      <c r="T120" t="n">
         <v>20</v>
       </c>
-      <c r="T120" t="n">
+      <c r="U120" t="n">
         <v>56</v>
       </c>
     </row>
     <row r="121">
-      <c r="S121" t="n">
+      <c r="T121" t="n">
         <v>20</v>
       </c>
-      <c r="T121" t="n">
+      <c r="U121" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="122">
-      <c r="S122" t="n">
+      <c r="T122" t="n">
         <v>22</v>
       </c>
-      <c r="T122" t="n">
+      <c r="U122" t="n">
         <v>66</v>
       </c>
     </row>
     <row r="123">
-      <c r="S123" t="n">
+      <c r="T123" t="n">
         <v>23</v>
       </c>
-      <c r="T123" t="n">
+      <c r="U123" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="124">
-      <c r="S124" t="n">
+      <c r="T124" t="n">
         <v>24</v>
       </c>
-      <c r="T124" t="n">
+      <c r="U124" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="125">
-      <c r="S125" t="n">
+      <c r="T125" t="n">
         <v>24</v>
       </c>
-      <c r="T125" t="n">
+      <c r="U125" t="n">
         <v>92</v>
       </c>
     </row>
     <row r="126">
-      <c r="S126" t="n">
+      <c r="T126" t="n">
         <v>24</v>
       </c>
-      <c r="T126" t="n">
+      <c r="U126" t="n">
         <v>93</v>
       </c>
     </row>
     <row r="127">
-      <c r="S127" t="n">
+      <c r="T127" t="n">
         <v>24</v>
       </c>
-      <c r="T127" t="n">
+      <c r="U127" t="n">
         <v>120</v>
       </c>
     </row>
     <row r="128">
-      <c r="S128" t="n">
+      <c r="T128" t="n">
         <v>25</v>
       </c>
-      <c r="T128" t="n">
+      <c r="U128" t="n">
         <v>85</v>
       </c>
     </row>
     <row r="133">
-      <c r="S133" t="s">
+      <c r="T133" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="134">
-      <c r="S134" t="s">
+      <c r="T134" t="s">
         <v>17</v>
       </c>
-      <c r="T134" t="s">
+      <c r="U134" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="135">
-      <c r="S135" t="n">
+      <c r="T135" t="n">
         <v>4</v>
       </c>
-      <c r="T135" t="n">
+      <c r="U135" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="136">
-      <c r="S136" t="n">
+      <c r="T136" t="n">
         <v>4</v>
       </c>
-      <c r="T136" t="n">
+      <c r="U136" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="137">
-      <c r="S137" t="n">
+      <c r="T137" t="n">
         <v>7</v>
       </c>
-      <c r="T137" t="n">
+      <c r="U137" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="138">
-      <c r="S138" t="n">
+      <c r="T138" t="n">
         <v>7</v>
       </c>
-      <c r="T138" t="n">
+      <c r="U138" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="139">
-      <c r="S139" t="n">
+      <c r="T139" t="n">
         <v>8</v>
       </c>
-      <c r="T139" t="n">
+      <c r="U139" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="140">
-      <c r="S140" t="n">
+      <c r="T140" t="n">
         <v>9</v>
       </c>
-      <c r="T140" t="n">
+      <c r="U140" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="141">
-      <c r="S141" t="n">
+      <c r="T141" t="n">
         <v>10</v>
       </c>
-      <c r="T141" t="n">
+      <c r="U141" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="142">
-      <c r="S142" t="n">
+      <c r="T142" t="n">
         <v>10</v>
       </c>
-      <c r="T142" t="n">
+      <c r="U142" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="143">
-      <c r="S143" t="n">
+      <c r="T143" t="n">
         <v>10</v>
       </c>
-      <c r="T143" t="n">
+      <c r="U143" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="144">
-      <c r="S144" t="n">
+      <c r="T144" t="n">
         <v>11</v>
       </c>
-      <c r="T144" t="n">
+      <c r="U144" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="145">
-      <c r="S145" t="n">
+      <c r="T145" t="n">
         <v>11</v>
       </c>
-      <c r="T145" t="n">
+      <c r="U145" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="146">
-      <c r="S146" t="n">
+      <c r="T146" t="n">
         <v>12</v>
       </c>
-      <c r="T146" t="n">
+      <c r="U146" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="147">
-      <c r="S147" t="n">
+      <c r="T147" t="n">
         <v>12</v>
       </c>
-      <c r="T147" t="n">
+      <c r="U147" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="148">
-      <c r="S148" t="n">
+      <c r="T148" t="n">
         <v>12</v>
       </c>
-      <c r="T148" t="n">
+      <c r="U148" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="149">
-      <c r="S149" t="n">
+      <c r="T149" t="n">
         <v>12</v>
       </c>
-      <c r="T149" t="n">
+      <c r="U149" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="150">
-      <c r="S150" t="n">
+      <c r="T150" t="n">
         <v>13</v>
       </c>
-      <c r="T150" t="n">
+      <c r="U150" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="151">
-      <c r="S151" t="n">
+      <c r="T151" t="n">
         <v>13</v>
       </c>
-      <c r="T151" t="n">
+      <c r="U151" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="152">
-      <c r="S152" t="n">
+      <c r="T152" t="n">
         <v>13</v>
       </c>
-      <c r="T152" t="n">
+      <c r="U152" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="153">
-      <c r="S153" t="n">
+      <c r="T153" t="n">
         <v>13</v>
       </c>
-      <c r="T153" t="n">
+      <c r="U153" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="154">
-      <c r="S154" t="n">
+      <c r="T154" t="n">
         <v>14</v>
       </c>
-      <c r="T154" t="n">
+      <c r="U154" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="155">
-      <c r="S155" t="n">
+      <c r="T155" t="n">
         <v>14</v>
       </c>
-      <c r="T155" t="n">
+      <c r="U155" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="156">
-      <c r="S156" t="n">
+      <c r="T156" t="n">
         <v>14</v>
       </c>
-      <c r="T156" t="n">
+      <c r="U156" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="157">
-      <c r="S157" t="n">
+      <c r="T157" t="n">
         <v>14</v>
       </c>
-      <c r="T157" t="n">
+      <c r="U157" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="158">
-      <c r="S158" t="n">
+      <c r="T158" t="n">
         <v>15</v>
       </c>
-      <c r="T158" t="n">
+      <c r="U158" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="159">
-      <c r="S159" t="n">
+      <c r="T159" t="n">
         <v>15</v>
       </c>
-      <c r="T159" t="n">
+      <c r="U159" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="160">
-      <c r="S160" t="n">
+      <c r="T160" t="n">
         <v>15</v>
       </c>
-      <c r="T160" t="n">
+      <c r="U160" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="161">
-      <c r="S161" t="n">
+      <c r="T161" t="n">
         <v>16</v>
       </c>
-      <c r="T161" t="n">
+      <c r="U161" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="162">
-      <c r="S162" t="n">
+      <c r="T162" t="n">
         <v>16</v>
       </c>
-      <c r="T162" t="n">
+      <c r="U162" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="163">
-      <c r="S163" t="n">
+      <c r="T163" t="n">
         <v>17</v>
       </c>
-      <c r="T163" t="n">
+      <c r="U163" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="164">
-      <c r="S164" t="n">
+      <c r="T164" t="n">
         <v>17</v>
       </c>
-      <c r="T164" t="n">
+      <c r="U164" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="165">
-      <c r="S165" t="n">
+      <c r="T165" t="n">
         <v>17</v>
       </c>
-      <c r="T165" t="n">
+      <c r="U165" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="166">
-      <c r="S166" t="n">
+      <c r="T166" t="n">
         <v>18</v>
       </c>
-      <c r="T166" t="n">
+      <c r="U166" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="167">
-      <c r="S167" t="n">
+      <c r="T167" t="n">
         <v>18</v>
       </c>
-      <c r="T167" t="n">
+      <c r="U167" t="n">
         <v>56</v>
       </c>
     </row>
     <row r="168">
-      <c r="S168" t="n">
+      <c r="T168" t="n">
         <v>18</v>
       </c>
-      <c r="T168" t="n">
+      <c r="U168" t="n">
         <v>76</v>
       </c>
     </row>
     <row r="169">
-      <c r="S169" t="n">
+      <c r="T169" t="n">
         <v>18</v>
       </c>
-      <c r="T169" t="n">
+      <c r="U169" t="n">
         <v>84</v>
       </c>
     </row>
     <row r="170">
-      <c r="S170" t="n">
+      <c r="T170" t="n">
         <v>19</v>
       </c>
-      <c r="T170" t="n">
+      <c r="U170" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="171">
-      <c r="S171" t="n">
+      <c r="T171" t="n">
         <v>19</v>
       </c>
-      <c r="T171" t="n">
+      <c r="U171" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="172">
-      <c r="S172" t="n">
+      <c r="T172" t="n">
         <v>19</v>
       </c>
-      <c r="T172" t="n">
+      <c r="U172" t="n">
         <v>68</v>
       </c>
     </row>
     <row r="173">
-      <c r="S173" t="n">
+      <c r="T173" t="n">
         <v>20</v>
       </c>
-      <c r="T173" t="n">
+      <c r="U173" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="174">
-      <c r="S174" t="n">
+      <c r="T174" t="n">
         <v>20</v>
       </c>
-      <c r="T174" t="n">
+      <c r="U174" t="n">
         <v>48</v>
       </c>
     </row>
     <row r="175">
-      <c r="S175" t="n">
+      <c r="T175" t="n">
         <v>20</v>
       </c>
-      <c r="T175" t="n">
+      <c r="U175" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="176">
-      <c r="S176" t="n">
+      <c r="T176" t="n">
         <v>20</v>
       </c>
-      <c r="T176" t="n">
+      <c r="U176" t="n">
         <v>56</v>
       </c>
     </row>
     <row r="177">
-      <c r="S177" t="n">
+      <c r="T177" t="n">
         <v>20</v>
       </c>
-      <c r="T177" t="n">
+      <c r="U177" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="178">
-      <c r="S178" t="n">
+      <c r="T178" t="n">
         <v>22</v>
       </c>
-      <c r="T178" t="n">
+      <c r="U178" t="n">
         <v>66</v>
       </c>
     </row>
     <row r="179">
-      <c r="S179" t="n">
+      <c r="T179" t="n">
         <v>23</v>
       </c>
-      <c r="T179" t="n">
+      <c r="U179" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="180">
-      <c r="S180" t="n">
+      <c r="T180" t="n">
         <v>24</v>
       </c>
-      <c r="T180" t="n">
+      <c r="U180" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="181">
-      <c r="S181" t="n">
+      <c r="T181" t="n">
         <v>24</v>
       </c>
-      <c r="T181" t="n">
+      <c r="U181" t="n">
         <v>92</v>
       </c>
     </row>
     <row r="182">
-      <c r="S182" t="n">
+      <c r="T182" t="n">
         <v>24</v>
       </c>
-      <c r="T182" t="n">
+      <c r="U182" t="n">
         <v>93</v>
       </c>
     </row>
     <row r="183">
-      <c r="S183" t="n">
+      <c r="T183" t="n">
         <v>24</v>
       </c>
-      <c r="T183" t="n">
+      <c r="U183" t="n">
         <v>120</v>
       </c>
     </row>
     <row r="184">
-      <c r="S184" t="n">
+      <c r="T184" t="n">
         <v>25</v>
       </c>
-      <c r="T184" t="n">
+      <c r="U184" t="n">
         <v>85</v>
       </c>
     </row>

</xml_diff>